<commit_message>
auf dem weg tabu suche ans laufen zu bekommen.
</commit_message>
<xml_diff>
--- a/output/localSearch 2015-03-03-15-05-53 Vergleich mit InnerTourMoves vs OhneInnerTourMoves.xlsx
+++ b/output/localSearch 2015-03-03-15-05-53 Vergleich mit InnerTourMoves vs OhneInnerTourMoves.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="localSearch 2015-03-03-15-05-53" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -1520,8 +1520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L58" sqref="L1:L58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>